<commit_message>
EPBDS-8218 fix representation of BigDecimal and BigDecimalValue with trailing zeros
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7973.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7973.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EIS_Sources\OpenL\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2CF2A7-7714-45B0-8A57-1E6116312E90}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D08F46-5FAF-4328-8F80-4ABB6F1F2403}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:D162"/>
+  <dimension ref="B4:D165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G153" sqref="G153"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,6 +751,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>4</v>
+      </c>
+    </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>14</v>
@@ -793,142 +798,155 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
-        <v>1</v>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>1</v>
-      </c>
-      <c r="C79">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B82" t="s">
-        <v>18</v>
+      <c r="B82">
+        <v>4</v>
+      </c>
+      <c r="C82">
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
-        <v>2</v>
+      <c r="B83">
+        <v>3</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B89" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B90" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B94" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B95" t="s">
-        <v>7</v>
-      </c>
-      <c r="C95" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B96">
-        <v>1</v>
-      </c>
-      <c r="C96">
-        <v>1</v>
-      </c>
-    </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B97">
-        <v>2</v>
-      </c>
-      <c r="C97">
-        <v>2</v>
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B98">
-        <v>3</v>
-      </c>
-      <c r="C98">
-        <v>3</v>
+      <c r="B98" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B99" s="1" t="s">
+      <c r="B99">
         <v>1</v>
       </c>
       <c r="C99">
@@ -936,7 +954,7 @@
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B100" s="1" t="s">
+      <c r="B100">
         <v>2</v>
       </c>
       <c r="C100">
@@ -944,90 +962,90 @@
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B101" s="1" t="s">
+      <c r="B101">
         <v>3</v>
       </c>
       <c r="C101">
         <v>3</v>
       </c>
     </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+    </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B103" t="s">
-        <v>21</v>
+      <c r="B103" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B104" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B105" t="s">
-        <v>2</v>
+      <c r="B104" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B110" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B111" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B115" t="s">
-        <v>7</v>
-      </c>
-      <c r="C115" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B116" t="s">
-        <v>7</v>
-      </c>
-      <c r="C116" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B117">
-        <v>1</v>
-      </c>
-      <c r="C117">
-        <v>1</v>
-      </c>
-    </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B118">
-        <v>2</v>
-      </c>
-      <c r="C118">
-        <v>2</v>
+      <c r="B118" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B119">
-        <v>3</v>
-      </c>
-      <c r="C119">
-        <v>3</v>
+      <c r="B119" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B120" s="1" t="s">
+      <c r="B120">
         <v>1</v>
       </c>
       <c r="C120">
@@ -1035,7 +1053,7 @@
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B121" s="1" t="s">
+      <c r="B121">
         <v>2</v>
       </c>
       <c r="C121">
@@ -1043,165 +1061,189 @@
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B122" s="1" t="s">
+      <c r="B122">
         <v>3</v>
       </c>
       <c r="C122">
         <v>3</v>
       </c>
     </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B123" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B124" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C124">
+        <v>2</v>
+      </c>
+    </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B125" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B126" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B127" t="s">
-        <v>2</v>
+      <c r="B125" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125">
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B132" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B133" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B137" t="s">
-        <v>7</v>
-      </c>
-      <c r="C137" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B138" t="s">
-        <v>7</v>
-      </c>
-      <c r="C138" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B139">
-        <v>1</v>
-      </c>
-      <c r="C139">
-        <v>1</v>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>7</v>
+      </c>
+      <c r="C140" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B141" t="s">
-        <v>27</v>
+        <v>7</v>
+      </c>
+      <c r="C141" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B142" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B143" t="s">
-        <v>2</v>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B144" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B148" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B149" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B155" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B153" t="s">
-        <v>7</v>
-      </c>
-      <c r="C153" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B154" t="s">
-        <v>7</v>
-      </c>
-      <c r="C154" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B155">
-        <v>1</v>
-      </c>
-      <c r="C155">
-        <v>1</v>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B156" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B157" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B158" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B159" t="s">
-        <v>7</v>
-      </c>
-      <c r="C159" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B160" t="s">
-        <v>7</v>
-      </c>
-      <c r="C160" t="s">
-        <v>8</v>
+      <c r="B158">
+        <v>1</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B161" t="s">
-        <v>1</v>
-      </c>
-      <c r="C161">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B162">
-        <v>2</v>
-      </c>
-      <c r="C162">
+      <c r="B162" t="s">
+        <v>7</v>
+      </c>
+      <c r="C162" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B163" t="s">
+        <v>7</v>
+      </c>
+      <c r="C163" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B164" t="s">
+        <v>1</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B165">
+        <v>2</v>
+      </c>
+      <c r="C165">
         <v>2</v>
       </c>
     </row>

</xml_diff>